<commit_message>
worked on monster properties
</commit_message>
<xml_diff>
--- a/Javascript - Beoordelingsformulier.xlsx
+++ b/Javascript - Beoordelingsformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BICT_edit\_Modules\Periode4\08_WEBS3\_WEBS3_1819\Toetsing\Beoordelings formulier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\webs3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57355389-4608-427F-B117-4344E987B81E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375F84CE-3D7A-4D1A-80E9-7E5DB5975449}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9270" yWindow="0" windowWidth="28080" windowHeight="8430" xr2:uid="{AA9A437F-FF9A-4A80-AC5C-35A5CB23D4D0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12810" xr2:uid="{AA9A437F-FF9A-4A80-AC5C-35A5CB23D4D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Javascript Beoordelingsform" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
   <si>
     <t>Examinator:</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Feedback / Motivatie</t>
   </si>
   <si>
-    <t>Student naam + Nummer</t>
-  </si>
-  <si>
     <t>Leerdoel(en):</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>Het is mogelijk tussen regio's te wisselen en daarbij de verschillende geplaatste monsters te zien. (onthouden van de locatie)</t>
+  </si>
+  <si>
+    <t>Simon Striekwold - 2137518</t>
   </si>
 </sst>
 </file>
@@ -1059,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0617BA-E293-4FAB-9924-AB67CB0C9515}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1080,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" t="s">
@@ -1095,29 +1095,29 @@
         <v>3</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="28"/>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D4" s="27"/>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D5" s="29"/>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1131,7 +1131,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1139,7 +1139,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1147,7 +1147,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1155,7 +1155,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1171,17 +1171,17 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="8" customFormat="1" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>13</v>
@@ -1207,10 +1207,10 @@
     </row>
     <row r="16" spans="1:8" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="12"/>
       <c r="E16" s="2"/>
@@ -1221,144 +1221,160 @@
     <row r="17" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="64"/>
       <c r="B17" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="33">
         <v>5</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="9"/>
+        <v>61</v>
+      </c>
+      <c r="F17" s="9">
+        <v>5</v>
+      </c>
       <c r="G17" s="19"/>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="64"/>
       <c r="B18" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="37">
         <v>3</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="F18" s="9">
+        <v>3</v>
+      </c>
       <c r="G18" s="19"/>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="64"/>
       <c r="B19" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="37">
         <v>3</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="F19" s="9">
+        <v>3</v>
+      </c>
       <c r="G19" s="19"/>
       <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="64"/>
       <c r="B20" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="41">
         <v>6</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="F20" s="9">
+        <v>6</v>
+      </c>
       <c r="G20" s="19"/>
       <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="64"/>
       <c r="B21" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="44">
         <v>3</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="F21" s="9">
+        <v>3</v>
+      </c>
       <c r="G21" s="19"/>
       <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="64"/>
       <c r="B22" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="37">
         <v>5</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="F22" s="9">
+        <v>5</v>
+      </c>
       <c r="G22" s="19"/>
       <c r="H22" s="11"/>
     </row>
     <row r="23" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="64"/>
       <c r="B23" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="41">
         <v>5</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="F23" s="9">
+        <v>5</v>
+      </c>
       <c r="G23" s="19"/>
       <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="64"/>
       <c r="B24" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" s="41">
         <v>8</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="9"/>
+        <v>64</v>
+      </c>
+      <c r="F24" s="9">
+        <v>8</v>
+      </c>
       <c r="G24" s="19"/>
       <c r="H24" s="12"/>
     </row>
@@ -1375,7 +1391,7 @@
     <row r="26" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="64"/>
       <c r="B26" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="56"/>
       <c r="D26" s="55"/>
@@ -1387,16 +1403,16 @@
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="64"/>
       <c r="B27" s="58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="60">
         <v>6</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="19"/>
@@ -1405,16 +1421,16 @@
     <row r="28" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="64"/>
       <c r="B28" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="37">
         <v>8</v>
       </c>
       <c r="E28" s="61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="19"/>
@@ -1423,34 +1439,36 @@
     <row r="29" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="64"/>
       <c r="B29" s="62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D29" s="37">
         <v>3</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="14"/>
+        <v>75</v>
+      </c>
+      <c r="F29" s="14">
+        <v>3</v>
+      </c>
       <c r="G29" s="19"/>
       <c r="H29" s="11"/>
     </row>
     <row r="30" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="64"/>
       <c r="B30" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" s="41">
         <v>8</v>
       </c>
       <c r="E30" s="42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="19"/>
@@ -1459,34 +1477,36 @@
     <row r="31" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="64"/>
       <c r="B31" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D31" s="37">
         <v>3</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="F31" s="9">
+        <v>3</v>
+      </c>
       <c r="G31" s="19"/>
       <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="64"/>
       <c r="B32" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" s="37">
         <v>9</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="19"/>
@@ -1505,34 +1525,36 @@
     <row r="34" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="64"/>
       <c r="B34" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="46">
         <v>10</v>
       </c>
       <c r="E34" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="F34" s="9">
+        <v>10</v>
+      </c>
       <c r="G34" s="9"/>
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="64"/>
       <c r="B35" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D35" s="46">
         <v>10</v>
       </c>
       <c r="E35" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="15"/>
@@ -1541,16 +1563,16 @@
     <row r="36" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="64"/>
       <c r="B36" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="46">
         <v>5</v>
       </c>
       <c r="E36" s="47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="19"/>
@@ -1570,7 +1592,10 @@
       <c r="E38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F38" s="19"/>
+      <c r="F38" s="19">
+        <f>SUM(F17:F37)</f>
+        <v>54</v>
+      </c>
       <c r="G38" s="21"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1580,12 +1605,9 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>20</v>
-      </c>
       <c r="B40"/>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
worked on monster powers
</commit_message>
<xml_diff>
--- a/Javascript - Beoordelingsformulier.xlsx
+++ b/Javascript - Beoordelingsformulier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\webs3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375F84CE-3D7A-4D1A-80E9-7E5DB5975449}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE15EC3-A492-4DEB-90A2-15F68B7177C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12810" xr2:uid="{AA9A437F-FF9A-4A80-AC5C-35A5CB23D4D0}"/>
   </bookViews>
@@ -1059,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0617BA-E293-4FAB-9924-AB67CB0C9515}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1432,9 @@
       <c r="E28" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="9"/>
+      <c r="F28" s="9">
+        <v>8</v>
+      </c>
       <c r="G28" s="19"/>
       <c r="H28" s="12"/>
     </row>
@@ -1594,7 +1596,7 @@
       </c>
       <c r="F38" s="19">
         <f>SUM(F17:F37)</f>
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G38" s="21"/>
     </row>

</xml_diff>